<commit_message>
commit curso de angular3
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Fecha</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>4.AppPiano 5.AppDatos 6.Componentes</t>
+  </si>
+  <si>
+    <t>7, App Tareas 8.App ConvertiorMonedas 9.Bmi calcultor</t>
   </si>
 </sst>
 </file>
@@ -193,16 +196,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -524,7 +527,7 @@
   <dimension ref="C2:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E8"/>
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,41 +557,47 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="9">
         <v>44729</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="3:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="9">
         <v>44732</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9">
+        <v>44733</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="3:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
@@ -596,259 +605,301 @@
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="3:5" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="3:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="3:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="3:5" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="3:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="3:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="3:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
     </row>
     <row r="44" spans="3:5" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
     </row>
     <row r="46" spans="3:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
     </row>
     <row r="52" spans="3:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="3:5" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -864,60 +915,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>